<commit_message>
tkinter solution on update
</commit_message>
<xml_diff>
--- a/python/test_gui/test_gui.xlsx
+++ b/python/test_gui/test_gui.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88215cb98efcb80/Documents/PythonTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC1048F1799D450A5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93D8FE6-3CCA-4B79-9D43-A8EA4DC8CEF2}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC1048F1799D450A5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29950254-D01D-4389-902B-567F1173AFB8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>key</t>
   </si>
@@ -48,9 +48,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>desc</t>
   </si>
   <si>
@@ -72,13 +69,28 @@
     <t>Another botton</t>
   </si>
   <si>
-    <t>button</t>
-  </si>
-  <si>
     <t>button1</t>
   </si>
   <si>
     <t>button2</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>The Log</t>
+  </si>
+  <si>
+    <t>Log box</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -140,6 +152,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -438,10 +454,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -452,38 +468,52 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>